<commit_message>
correlation analysis completed for the variables
</commit_message>
<xml_diff>
--- a/data/Report - Data Tables Ver4_Fin_SA 072724.xlsx
+++ b/data/Report - Data Tables Ver4_Fin_SA 072724.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sifaat\FFC-Forecasting-Study\Lit-Review+Inception-Report\FFC-Inception_Reports-Submission-files\FFC-Inception_Reports-Submission-files\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sifaat\FFC-Forecasting-Study\forecasting-study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D12233-8082-42B9-99B3-7661083EE9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4009FFA6-1037-443F-B372-171EC79B290C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Consolidated" sheetId="3" r:id="rId1"/>
@@ -531,9 +531,6 @@
     <t>GDP (current US$) C-Y (BN$)</t>
   </si>
   <si>
-    <t>Aricultural GDP (current US$) C-Y</t>
-  </si>
-  <si>
     <t>Table 4.3</t>
   </si>
   <si>
@@ -559,6 +556,9 @@
   </si>
   <si>
     <t>Agricultural  GDP in USD</t>
+  </si>
+  <si>
+    <t>Agricultural GDP (current US$) C-Y</t>
   </si>
 </sst>
 </file>
@@ -1468,31 +1468,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1506,6 +1481,31 @@
     <xf numFmtId="166" fontId="21" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1729,8 +1729,8 @@
   </sheetPr>
   <dimension ref="B1:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1764,13 +1764,13 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="203" t="s">
+      <c r="H2" s="213" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="203"/>
-      <c r="J2" s="204"/>
-      <c r="K2" s="204"/>
-      <c r="L2" s="204"/>
+      <c r="I2" s="213"/>
+      <c r="J2" s="214"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="214"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
@@ -3333,17 +3333,17 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="2:11" ht="18">
-      <c r="C2" s="209" t="s">
+      <c r="C2" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="209"/>
-      <c r="E2" s="209"/>
-      <c r="F2" s="209"/>
-      <c r="G2" s="209"/>
-      <c r="H2" s="209"/>
-      <c r="I2" s="209"/>
-      <c r="J2" s="209"/>
-      <c r="K2" s="209"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="219"/>
+      <c r="K2" s="219"/>
     </row>
     <row r="3" spans="2:11" ht="14.4">
       <c r="C3" s="15" t="s">
@@ -4698,36 +4698,36 @@
       <c r="X1" s="18"/>
     </row>
     <row r="2" spans="2:29" ht="18">
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="220" t="s">
         <v>158</v>
       </c>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="210"/>
-      <c r="P2" s="210"/>
-      <c r="Q2" s="210"/>
-      <c r="R2" s="210"/>
-      <c r="S2" s="210"/>
-      <c r="T2" s="210"/>
-      <c r="U2" s="210"/>
-      <c r="V2" s="210"/>
-      <c r="W2" s="210"/>
-      <c r="X2" s="210"/>
-      <c r="Z2" s="208" t="s">
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
+      <c r="M2" s="220"/>
+      <c r="N2" s="220"/>
+      <c r="O2" s="220"/>
+      <c r="P2" s="220"/>
+      <c r="Q2" s="220"/>
+      <c r="R2" s="220"/>
+      <c r="S2" s="220"/>
+      <c r="T2" s="220"/>
+      <c r="U2" s="220"/>
+      <c r="V2" s="220"/>
+      <c r="W2" s="220"/>
+      <c r="X2" s="220"/>
+      <c r="Z2" s="217" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="208"/>
-      <c r="AB2" s="208"/>
-      <c r="AC2" s="208"/>
+      <c r="AA2" s="217"/>
+      <c r="AB2" s="217"/>
+      <c r="AC2" s="217"/>
     </row>
     <row r="3" spans="2:29" ht="14.4">
       <c r="C3" s="27" t="s">
@@ -17468,14 +17468,14 @@
       <c r="D1" s="14"/>
     </row>
     <row r="2" spans="2:7" ht="18">
-      <c r="B2" s="208" t="s">
+      <c r="B2" s="217" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
     </row>
     <row r="3" spans="2:7" ht="18">
       <c r="B3" s="95"/>
@@ -18293,13 +18293,13 @@
       <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="208" t="s">
+      <c r="A2" s="217" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
     </row>
     <row r="3" spans="1:5" s="25" customFormat="1" ht="14.4">
       <c r="C3" s="28" t="s">
@@ -18747,11 +18747,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="14.4">
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="221" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
     </row>
     <row r="4" spans="2:4" ht="43.2">
       <c r="B4" s="34" t="s">
@@ -19171,11 +19171,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="14.4">
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="221" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
     </row>
     <row r="4" spans="2:4" ht="57.6">
       <c r="B4" s="34" t="s">
@@ -19598,12 +19598,12 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="18">
-      <c r="C3" s="205" t="s">
+      <c r="C3" s="215" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="205"/>
-      <c r="E3" s="205"/>
-      <c r="F3" s="205"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
     </row>
     <row r="4" spans="2:6" ht="14.4">
       <c r="C4" s="17" t="s">
@@ -23186,14 +23186,14 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="18">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="215" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="205"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="205"/>
-      <c r="E3" s="205"/>
-      <c r="F3" s="205"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
     </row>
     <row r="4" spans="1:6" ht="14.4">
       <c r="C4" s="17" t="s">
@@ -23727,8 +23727,8 @@
   </sheetPr>
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:Z3"/>
+    <sheetView topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -23759,38 +23759,38 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:27" ht="18">
-      <c r="C3" s="205" t="s">
+      <c r="C3" s="215" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="205"/>
-      <c r="E3" s="205"/>
-      <c r="F3" s="205"/>
-      <c r="I3" s="205" t="s">
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
+      <c r="I3" s="215" t="s">
         <v>121</v>
       </c>
-      <c r="J3" s="205"/>
-      <c r="K3" s="205"/>
-      <c r="N3" s="208" t="s">
+      <c r="J3" s="215"/>
+      <c r="K3" s="215"/>
+      <c r="N3" s="217" t="s">
+        <v>172</v>
+      </c>
+      <c r="O3" s="217"/>
+      <c r="P3" s="217"/>
+      <c r="S3" s="217" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="208"/>
-      <c r="P3" s="208"/>
-      <c r="S3" s="208" t="s">
-        <v>174</v>
-      </c>
-      <c r="T3" s="208"/>
-      <c r="U3" s="208"/>
-      <c r="V3" s="208"/>
-      <c r="W3" s="208"/>
-      <c r="X3" s="208"/>
-      <c r="Y3" s="208"/>
-      <c r="Z3" s="208"/>
+      <c r="T3" s="217"/>
+      <c r="U3" s="217"/>
+      <c r="V3" s="217"/>
+      <c r="W3" s="217"/>
+      <c r="X3" s="217"/>
+      <c r="Y3" s="217"/>
+      <c r="Z3" s="217"/>
     </row>
     <row r="4" spans="1:27" ht="14.4">
-      <c r="B4" s="206" t="s">
+      <c r="B4" s="216" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="206"/>
+      <c r="C4" s="216"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="I4" s="55" t="s">
@@ -23798,10 +23798,10 @@
       </c>
       <c r="J4" s="55"/>
       <c r="M4" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="R4" s="55" t="s">
         <v>166</v>
-      </c>
-      <c r="R4" s="55" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="57.6">
@@ -23825,7 +23825,7 @@
       </c>
       <c r="H5" s="57"/>
       <c r="I5" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J5" s="34" t="s">
         <v>120</v>
@@ -23861,19 +23861,19 @@
         <v>118</v>
       </c>
       <c r="W5" s="34" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="X5" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y5" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z5" s="218" t="str">
+        <v>169</v>
+      </c>
+      <c r="Z5" s="209" t="str">
         <f>O5</f>
         <v>PKR per USD*</v>
       </c>
-      <c r="AA5" s="218" t="str">
+      <c r="AA5" s="209" t="str">
         <f>P5</f>
         <v>Rate of Change in Forex PKR/USD</v>
       </c>
@@ -23901,7 +23901,7 @@
       </c>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
-      <c r="K6" s="219">
+      <c r="K6" s="210">
         <f>E6/G6</f>
         <v>0.1448726322664925</v>
       </c>
@@ -23928,11 +23928,11 @@
         <f>T6/1000000000</f>
         <v>52.293470813133595</v>
       </c>
-      <c r="V6" s="212">
-        <f>K6</f>
+      <c r="V6" s="203">
+        <f t="shared" ref="V6:V35" si="1">K6</f>
         <v>0.1448726322664925</v>
       </c>
-      <c r="W6" s="220">
+      <c r="W6" s="211">
         <f>T6*V6</f>
         <v>7575892767.0496626</v>
       </c>
@@ -23942,10 +23942,10 @@
       </c>
       <c r="Y6" s="32"/>
       <c r="Z6" s="32">
-        <f t="shared" ref="Z6:Z35" si="1">O6</f>
+        <f t="shared" ref="Z6:Z35" si="2">O6</f>
         <v>30.163799999999998</v>
       </c>
-      <c r="AA6" s="213"/>
+      <c r="AA6" s="204"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="B7" s="102">
@@ -23966,7 +23966,7 @@
         <v>1671977</v>
       </c>
       <c r="G7" s="56">
-        <f t="shared" ref="G7:G35" si="2">F7/1000</f>
+        <f t="shared" ref="G7:G35" si="3">F7/1000</f>
         <v>1671.9770000000001</v>
       </c>
       <c r="I7" s="84">
@@ -23977,8 +23977,8 @@
         <f>((F7/F6)-1)</f>
         <v>0.19353185353335256</v>
       </c>
-      <c r="K7" s="219">
-        <f t="shared" ref="K7:K35" si="3">E7/G7</f>
+      <c r="K7" s="210">
+        <f t="shared" ref="K7:K35" si="4">E7/G7</f>
         <v>0.14951820509492655</v>
       </c>
       <c r="M7" s="122">
@@ -24006,37 +24006,37 @@
         <v>60636071684.191803</v>
       </c>
       <c r="U7" s="69">
-        <f t="shared" ref="U7:U35" si="4">T7/1000000000</f>
+        <f t="shared" ref="U7:U35" si="5">T7/1000000000</f>
         <v>60.636071684191805</v>
       </c>
-      <c r="V7" s="212">
-        <f>K7</f>
+      <c r="V7" s="203">
+        <f t="shared" si="1"/>
         <v>0.14951820509492655</v>
       </c>
-      <c r="W7" s="220">
-        <f t="shared" ref="W7:W35" si="5">T7*V7</f>
+      <c r="W7" s="211">
+        <f t="shared" ref="W7:W35" si="6">T7*V7</f>
         <v>9066196602.2276592</v>
       </c>
       <c r="X7" s="69">
-        <f t="shared" ref="X7:X35" si="6">W7/1000000000</f>
+        <f t="shared" ref="X7:X35" si="7">W7/1000000000</f>
         <v>9.0661966022276594</v>
       </c>
       <c r="Y7" s="84">
         <f>((X7/X6)-1)</f>
         <v>0.19671659578655531</v>
       </c>
-      <c r="Z7" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z7" s="205">
+        <f t="shared" si="2"/>
         <v>30.8507</v>
       </c>
-      <c r="AA7" s="215">
+      <c r="AA7" s="206">
         <f>P7</f>
         <v>2.2772329746252096E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="B8" s="102">
-        <f t="shared" ref="B8:B35" si="7">B7+1</f>
+        <f t="shared" ref="B8:B35" si="8">B7+1</f>
         <v>3</v>
       </c>
       <c r="C8" s="99" t="s">
@@ -24053,19 +24053,19 @@
         <v>1929891</v>
       </c>
       <c r="G8" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1929.8910000000001</v>
       </c>
       <c r="I8" s="81">
-        <f t="shared" ref="I8:I35" si="8">((D8/D7)-1)</f>
+        <f t="shared" ref="I8:I35" si="9">((D8/D7)-1)</f>
         <v>0.11168402062474247</v>
       </c>
       <c r="J8" s="81">
-        <f t="shared" ref="J8:J35" si="9">((F8/F7)-1)</f>
+        <f t="shared" ref="J8:J35" si="10">((F8/F7)-1)</f>
         <v>0.15425690664405067</v>
       </c>
-      <c r="K8" s="219">
-        <f t="shared" si="3"/>
+      <c r="K8" s="210">
+        <f t="shared" si="4"/>
         <v>0.14400346962600477</v>
       </c>
       <c r="M8" s="122">
@@ -24079,7 +24079,7 @@
         <v>33.568399999999997</v>
       </c>
       <c r="P8" s="93">
-        <f t="shared" ref="P8:P35" si="10">((O8/O7)-1)</f>
+        <f t="shared" ref="P8:P35" si="11">((O8/O7)-1)</f>
         <v>8.8092004395362133E-2</v>
       </c>
       <c r="R8" s="122">
@@ -24093,37 +24093,37 @@
         <v>63320170084.4076</v>
       </c>
       <c r="U8" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63.3201700844076</v>
       </c>
-      <c r="V8" s="212">
-        <f>K8</f>
+      <c r="V8" s="203">
+        <f t="shared" si="1"/>
         <v>0.14400346962600477</v>
       </c>
-      <c r="W8" s="220">
-        <f t="shared" si="5"/>
+      <c r="W8" s="211">
+        <f t="shared" si="6"/>
         <v>9118324189.4634457</v>
       </c>
       <c r="X8" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.1183241894634453</v>
       </c>
       <c r="Y8" s="81">
-        <f t="shared" ref="Y8:Y35" si="11">((X8/X7)-1)</f>
+        <f t="shared" ref="Y8:Y35" si="12">((X8/X7)-1)</f>
         <v>5.7496643325578578E-3</v>
       </c>
       <c r="Z8" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.568399999999997</v>
       </c>
-      <c r="AA8" s="213">
-        <f t="shared" ref="AA8:AA35" si="12">P8</f>
+      <c r="AA8" s="204">
+        <f t="shared" ref="AA8:AA35" si="13">P8</f>
         <v>8.8092004395362133E-2</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="B9" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="C9" s="99" t="s">
@@ -24140,23 +24140,23 @@
         <v>2226580</v>
       </c>
       <c r="G9" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2226.58</v>
       </c>
       <c r="I9" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.7283338910658426E-2</v>
       </c>
       <c r="J9" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.15373355282759493</v>
       </c>
-      <c r="K9" s="219">
-        <f t="shared" si="3"/>
+      <c r="K9" s="210">
+        <f t="shared" si="4"/>
         <v>0.1357094737220311</v>
       </c>
       <c r="M9" s="122">
-        <f t="shared" ref="M9:M35" si="13">M8+1</f>
+        <f t="shared" ref="M9:M35" si="14">M8+1</f>
         <v>4</v>
       </c>
       <c r="N9" s="123" t="s">
@@ -24166,11 +24166,11 @@
         <v>38.993600000000001</v>
       </c>
       <c r="P9" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.16161628197948086</v>
       </c>
       <c r="R9" s="122">
-        <f t="shared" ref="R9:R35" si="14">R8+1</f>
+        <f t="shared" ref="R9:R35" si="15">R8+1</f>
         <v>4</v>
       </c>
       <c r="S9" s="123" t="s">
@@ -24180,37 +24180,37 @@
         <v>62433340468.022797</v>
       </c>
       <c r="U9" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.433340468022799</v>
       </c>
-      <c r="V9" s="212">
-        <f>K9</f>
+      <c r="V9" s="203">
+        <f t="shared" si="1"/>
         <v>0.1357094737220311</v>
       </c>
-      <c r="W9" s="220">
-        <f t="shared" si="5"/>
+      <c r="W9" s="211">
+        <f t="shared" si="6"/>
         <v>8472795777.6237602</v>
       </c>
       <c r="X9" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.4727957776237606</v>
       </c>
       <c r="Y9" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-7.0794632700778126E-2</v>
       </c>
       <c r="Z9" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38.993600000000001</v>
       </c>
-      <c r="AA9" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA9" s="204">
+        <f t="shared" si="13"/>
         <v>0.16161628197948086</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="B10" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="C10" s="99" t="s">
@@ -24227,24 +24227,24 @@
         <v>2480884</v>
       </c>
       <c r="G10" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2480.884</v>
       </c>
       <c r="I10" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.21391742342008424</v>
       </c>
       <c r="J10" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.11421282864303106</v>
       </c>
-      <c r="K10" s="219">
-        <f t="shared" si="3"/>
+      <c r="K10" s="210">
+        <f t="shared" si="4"/>
         <v>0.14785334582350484</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="N10" s="123" t="s">
@@ -24254,12 +24254,12 @@
         <v>43.195799999999998</v>
       </c>
       <c r="P10" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10776640269172377</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="S10" s="123" t="s">
@@ -24269,37 +24269,37 @@
         <v>62191955814.347801</v>
       </c>
       <c r="U10" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.1919558143478</v>
       </c>
-      <c r="V10" s="212">
-        <f>K10</f>
+      <c r="V10" s="203">
+        <f t="shared" si="1"/>
         <v>0.14785334582350484</v>
       </c>
-      <c r="W10" s="220">
-        <f t="shared" si="5"/>
+      <c r="W10" s="211">
+        <f t="shared" si="6"/>
         <v>9195288750.4588985</v>
       </c>
       <c r="X10" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.1952887504588983</v>
       </c>
       <c r="Y10" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.5272086309834849E-2</v>
       </c>
-      <c r="Z10" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z10" s="205">
+        <f t="shared" si="2"/>
         <v>43.195799999999998</v>
       </c>
-      <c r="AA10" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA10" s="206">
+        <f t="shared" si="13"/>
         <v>0.10776640269172377</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15.6" customHeight="1">
       <c r="B11" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="C11" s="99" t="s">
@@ -24316,23 +24316,23 @@
         <v>2735943</v>
       </c>
       <c r="G11" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2735.9430000000002</v>
       </c>
       <c r="I11" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.8820360571090449E-2</v>
       </c>
       <c r="J11" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.10280972427570179</v>
       </c>
-      <c r="K11" s="219">
-        <f t="shared" si="3"/>
+      <c r="K11" s="210">
+        <f t="shared" si="4"/>
         <v>0.14731849311188133</v>
       </c>
       <c r="M11" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="N11" s="123" t="s">
@@ -24342,11 +24342,11 @@
         <v>50.054600000000001</v>
       </c>
       <c r="P11" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.15878395584755922</v>
       </c>
       <c r="R11" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="S11" s="123" t="s">
@@ -24356,37 +24356,37 @@
         <v>62973857068.511299</v>
       </c>
       <c r="U11" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.9738570685113</v>
       </c>
-      <c r="V11" s="212">
-        <f>K11</f>
+      <c r="V11" s="203">
+        <f t="shared" si="1"/>
         <v>0.14731849311188133</v>
       </c>
-      <c r="W11" s="220">
-        <f t="shared" si="5"/>
+      <c r="W11" s="211">
+        <f t="shared" si="6"/>
         <v>9277213728.7760811</v>
       </c>
       <c r="X11" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.277213728776081</v>
       </c>
       <c r="Y11" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.9094514093528421E-3</v>
       </c>
       <c r="Z11" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50.054600000000001</v>
       </c>
-      <c r="AA11" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA11" s="204">
+        <f t="shared" si="13"/>
         <v>0.15878395584755922</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="25.8" customHeight="1">
       <c r="B12" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="C12" s="99" t="s">
@@ -24403,26 +24403,26 @@
         <v>4870957</v>
       </c>
       <c r="G12" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4870.9570000000003</v>
       </c>
       <c r="I12" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.5681135328925333</v>
       </c>
       <c r="J12" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.78035763171966677</v>
       </c>
-      <c r="K12" s="219">
-        <f t="shared" si="3"/>
+      <c r="K12" s="210">
+        <f t="shared" si="4"/>
         <v>0.1297560212500336</v>
       </c>
-      <c r="L12" s="221" t="s">
+      <c r="L12" s="212" t="s">
         <v>143</v>
       </c>
       <c r="M12" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="N12" s="123" t="s">
@@ -24432,11 +24432,11 @@
         <v>51.770899999999997</v>
       </c>
       <c r="P12" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.4288556895869737E-2</v>
       </c>
       <c r="R12" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="S12" s="123" t="s">
@@ -24446,37 +24446,37 @@
         <v>99484802344.527695</v>
       </c>
       <c r="U12" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99.484802344527694</v>
       </c>
-      <c r="V12" s="212">
-        <f>K12</f>
+      <c r="V12" s="203">
+        <f t="shared" si="1"/>
         <v>0.1297560212500336</v>
       </c>
-      <c r="W12" s="220">
-        <f t="shared" si="5"/>
+      <c r="W12" s="211">
+        <f t="shared" si="6"/>
         <v>12908752127.071928</v>
       </c>
       <c r="X12" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12.908752127071928</v>
       </c>
       <c r="Y12" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.39144709871580652</v>
       </c>
-      <c r="Z12" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z12" s="205">
+        <f t="shared" si="2"/>
         <v>51.770899999999997</v>
       </c>
-      <c r="AA12" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA12" s="206">
+        <f t="shared" si="13"/>
         <v>3.4288556895869737E-2</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="B13" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="C13" s="100">
@@ -24493,23 +24493,23 @@
         <v>5356237</v>
       </c>
       <c r="G13" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5356.2370000000001</v>
       </c>
       <c r="I13" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-7.3366074084387778E-3</v>
       </c>
       <c r="J13" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.9627239575303062E-2</v>
       </c>
-      <c r="K13" s="219">
-        <f t="shared" si="3"/>
+      <c r="K13" s="210">
+        <f t="shared" si="4"/>
         <v>0.11713428662697338</v>
       </c>
       <c r="M13" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="N13" s="123" t="s">
@@ -24519,11 +24519,11 @@
         <v>58.437800000000003</v>
       </c>
       <c r="P13" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.12877697702763524</v>
       </c>
       <c r="R13" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="S13" s="123" t="s">
@@ -24533,37 +24533,37 @@
         <v>97145618479.903793</v>
       </c>
       <c r="U13" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97.145618479903789</v>
       </c>
-      <c r="V13" s="212">
-        <f>K13</f>
+      <c r="V13" s="203">
+        <f t="shared" si="1"/>
         <v>0.11713428662697338</v>
       </c>
-      <c r="W13" s="220">
-        <f t="shared" si="5"/>
+      <c r="W13" s="211">
+        <f t="shared" si="6"/>
         <v>11379082719.579653</v>
       </c>
       <c r="X13" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.379082719579653</v>
       </c>
       <c r="Y13" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.11849862732155869</v>
       </c>
       <c r="Z13" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.437800000000003</v>
       </c>
-      <c r="AA13" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA13" s="204">
+        <f t="shared" si="13"/>
         <v>0.12877697702763524</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="B14" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="C14" s="100">
@@ -24580,23 +24580,23 @@
         <v>5710892</v>
       </c>
       <c r="G14" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5710.8919999999998</v>
       </c>
       <c r="I14" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.7739954956893427E-2</v>
       </c>
       <c r="J14" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.6213462921823618E-2</v>
       </c>
-      <c r="K14" s="219">
-        <f t="shared" si="3"/>
+      <c r="K14" s="210">
+        <f t="shared" si="4"/>
         <v>0.10461535605996401</v>
       </c>
       <c r="M14" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="N14" s="123" t="s">
@@ -24606,11 +24606,11 @@
         <v>61.425800000000002</v>
       </c>
       <c r="P14" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.1131288309963718E-2</v>
       </c>
       <c r="R14" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9</v>
       </c>
       <c r="S14" s="123" t="s">
@@ -24620,31 +24620,31 @@
         <v>97923302809.353699</v>
       </c>
       <c r="U14" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97.9233028093537</v>
       </c>
-      <c r="V14" s="212">
-        <f>K14</f>
+      <c r="V14" s="203">
+        <f t="shared" si="1"/>
         <v>0.10461535605996401</v>
       </c>
-      <c r="W14" s="220">
-        <f t="shared" si="5"/>
+      <c r="W14" s="211">
+        <f t="shared" si="6"/>
         <v>10244281189.968212</v>
       </c>
       <c r="X14" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10.244281189968213</v>
       </c>
       <c r="Y14" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-9.9726977786954718E-2</v>
       </c>
       <c r="Z14" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61.425800000000002</v>
       </c>
-      <c r="AA14" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA14" s="204">
+        <f t="shared" si="13"/>
         <v>5.1131288309963718E-2</v>
       </c>
     </row>
@@ -24653,7 +24653,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="C15" s="100">
@@ -24670,23 +24670,23 @@
         <v>6218516</v>
       </c>
       <c r="G15" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6218.5159999999996</v>
       </c>
       <c r="I15" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.43621944708066E-2</v>
       </c>
       <c r="J15" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.8886989983351095E-2</v>
       </c>
-      <c r="K15" s="219">
-        <f t="shared" si="3"/>
+      <c r="K15" s="210">
+        <f t="shared" si="4"/>
         <v>0.10225912420262326</v>
       </c>
       <c r="M15" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="N15" s="123" t="s">
@@ -24696,11 +24696,11 @@
         <v>58.499499999999998</v>
       </c>
       <c r="P15" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-4.7639591181555696E-2</v>
       </c>
       <c r="R15" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="S15" s="123" t="s">
@@ -24710,37 +24710,37 @@
         <v>112371913740.823</v>
       </c>
       <c r="U15" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>112.371913740823</v>
       </c>
-      <c r="V15" s="212">
-        <f>K15</f>
+      <c r="V15" s="203">
+        <f t="shared" si="1"/>
         <v>0.10225912420262326</v>
       </c>
-      <c r="W15" s="220">
-        <f t="shared" si="5"/>
+      <c r="W15" s="211">
+        <f t="shared" si="6"/>
         <v>11491053484.109285</v>
       </c>
       <c r="X15" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.491053484109285</v>
       </c>
       <c r="Y15" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.12170422414429449</v>
       </c>
       <c r="Z15" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58.499499999999998</v>
       </c>
-      <c r="AA15" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA15" s="204">
+        <f t="shared" si="13"/>
         <v>-4.7639591181555696E-2</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="B16" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="C16" s="100">
@@ -24757,23 +24757,23 @@
         <v>7198417</v>
       </c>
       <c r="G16" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7198.4170000000004</v>
       </c>
       <c r="I16" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.17617392671803733</v>
       </c>
       <c r="J16" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.15757794946575676</v>
       </c>
-      <c r="K16" s="219">
-        <f t="shared" si="3"/>
+      <c r="K16" s="210">
+        <f t="shared" si="4"/>
         <v>0.10390187175874917</v>
       </c>
       <c r="M16" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="N16" s="123" t="s">
@@ -24783,11 +24783,11 @@
         <v>57.5745</v>
       </c>
       <c r="P16" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.5812100958127795E-2</v>
       </c>
       <c r="R16" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="S16" s="123" t="s">
@@ -24797,37 +24797,37 @@
         <v>132216048339.41299</v>
       </c>
       <c r="U16" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>132.21604833941299</v>
       </c>
-      <c r="V16" s="212">
-        <f>K16</f>
+      <c r="V16" s="203">
+        <f t="shared" si="1"/>
         <v>0.10390187175874917</v>
       </c>
-      <c r="W16" s="220">
-        <f t="shared" si="5"/>
+      <c r="W16" s="211">
+        <f t="shared" si="6"/>
         <v>13737494899.010269</v>
       </c>
       <c r="X16" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.737494899010269</v>
       </c>
       <c r="Y16" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.19549481846964989</v>
       </c>
       <c r="Z16" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57.5745</v>
       </c>
-      <c r="AA16" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA16" s="204">
+        <f t="shared" si="13"/>
         <v>-1.5812100958127795E-2</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="15.75" customHeight="1">
       <c r="B17" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="C17" s="100">
@@ -24844,23 +24844,23 @@
         <v>8211010</v>
       </c>
       <c r="G17" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8211.01</v>
       </c>
       <c r="I17" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.6870157461470319E-2</v>
       </c>
       <c r="J17" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.14066884427506765</v>
       </c>
-      <c r="K17" s="219">
-        <f t="shared" si="3"/>
+      <c r="K17" s="210">
+        <f t="shared" si="4"/>
         <v>9.9912312857979704E-2</v>
       </c>
       <c r="M17" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="N17" s="123" t="s">
@@ -24870,11 +24870,11 @@
         <v>59.357599999999998</v>
       </c>
       <c r="P17" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.0970308035675576E-2</v>
       </c>
       <c r="R17" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="S17" s="123" t="s">
@@ -24884,37 +24884,37 @@
         <v>145208562960.767</v>
       </c>
       <c r="U17" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>145.20856296076701</v>
       </c>
-      <c r="V17" s="212">
-        <f>K17</f>
+      <c r="V17" s="203">
+        <f t="shared" si="1"/>
         <v>9.9912312857979704E-2</v>
       </c>
-      <c r="W17" s="220">
-        <f t="shared" si="5"/>
+      <c r="W17" s="211">
+        <f t="shared" si="6"/>
         <v>14508123372.193796</v>
       </c>
       <c r="X17" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.508123372193797</v>
       </c>
       <c r="Y17" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.6096724974147083E-2</v>
       </c>
       <c r="Z17" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59.357599999999998</v>
       </c>
-      <c r="AA17" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA17" s="204">
+        <f t="shared" si="13"/>
         <v>3.0970308035675576E-2</v>
       </c>
     </row>
     <row r="18" spans="2:27" ht="15.75" customHeight="1">
       <c r="B18" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="C18" s="100">
@@ -24931,23 +24931,23 @@
         <v>9188688</v>
       </c>
       <c r="G18" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9188.6880000000001</v>
       </c>
       <c r="I18" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1208206918492669E-2</v>
       </c>
       <c r="J18" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.11906915227237569</v>
       </c>
-      <c r="K18" s="219">
-        <f t="shared" si="3"/>
+      <c r="K18" s="210">
+        <f t="shared" si="4"/>
         <v>9.028231233882357E-2</v>
       </c>
       <c r="M18" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="N18" s="123" t="s">
@@ -24957,11 +24957,11 @@
         <v>59.8566</v>
       </c>
       <c r="P18" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8.4066741242907472E-3</v>
       </c>
       <c r="R18" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>13</v>
       </c>
       <c r="S18" s="123" t="s">
@@ -24971,37 +24971,37 @@
         <v>161871385506.35999</v>
       </c>
       <c r="U18" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>161.87138550635999</v>
       </c>
-      <c r="V18" s="212">
-        <f>K18</f>
+      <c r="V18" s="203">
+        <f t="shared" si="1"/>
         <v>9.028231233882357E-2</v>
       </c>
-      <c r="W18" s="220">
-        <f t="shared" si="5"/>
+      <c r="W18" s="211">
+        <f t="shared" si="6"/>
         <v>14614122985.003311</v>
       </c>
       <c r="X18" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14.614122985003311</v>
       </c>
       <c r="Y18" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.3062249396549372E-3</v>
       </c>
       <c r="Z18" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59.8566</v>
       </c>
-      <c r="AA18" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA18" s="204">
+        <f t="shared" si="13"/>
         <v>8.4066741242907472E-3</v>
       </c>
     </row>
     <row r="19" spans="2:27" ht="15.75" customHeight="1">
       <c r="B19" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="C19" s="100">
@@ -25018,23 +25018,23 @@
         <v>10661214</v>
       </c>
       <c r="G19" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10661.214</v>
       </c>
       <c r="I19" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.16194779019643768</v>
       </c>
       <c r="J19" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.16025421692411368</v>
       </c>
-      <c r="K19" s="219">
-        <f t="shared" si="3"/>
+      <c r="K19" s="210">
+        <f t="shared" si="4"/>
         <v>9.0414093554448863E-2</v>
       </c>
       <c r="M19" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="N19" s="123" t="s">
@@ -25044,11 +25044,11 @@
         <v>60.6342</v>
       </c>
       <c r="P19" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.2991048606168842E-2</v>
       </c>
       <c r="R19" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>14</v>
       </c>
       <c r="S19" s="123" t="s">
@@ -25058,37 +25058,37 @@
         <v>184140869997.45999</v>
       </c>
       <c r="U19" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>184.14086999745999</v>
       </c>
-      <c r="V19" s="212">
-        <f>K19</f>
+      <c r="V19" s="203">
+        <f t="shared" si="1"/>
         <v>9.0414093554448863E-2</v>
       </c>
-      <c r="W19" s="220">
-        <f t="shared" si="5"/>
+      <c r="W19" s="211">
+        <f t="shared" si="6"/>
         <v>16648929847.147953</v>
       </c>
       <c r="X19" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.648929847147954</v>
       </c>
       <c r="Y19" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.13923564652033638</v>
       </c>
       <c r="Z19" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60.6342</v>
       </c>
-      <c r="AA19" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA19" s="204">
+        <f t="shared" si="13"/>
         <v>1.2991048606168842E-2</v>
       </c>
     </row>
     <row r="20" spans="2:27" ht="15.75" customHeight="1">
       <c r="B20" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="C20" s="100">
@@ -25105,23 +25105,23 @@
         <v>12364620</v>
       </c>
       <c r="G20" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12364.62</v>
       </c>
       <c r="I20" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19883206559853273</v>
       </c>
       <c r="J20" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.15977598798785952</v>
       </c>
-      <c r="K20" s="219">
-        <f t="shared" si="3"/>
+      <c r="K20" s="210">
+        <f t="shared" si="4"/>
         <v>9.3458836583736507E-2</v>
       </c>
       <c r="M20" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="N20" s="123" t="s">
@@ -25131,11 +25131,11 @@
         <v>62.546500000000002</v>
       </c>
       <c r="P20" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.1538306764169466E-2</v>
       </c>
       <c r="R20" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
       <c r="S20" s="123" t="s">
@@ -25145,37 +25145,37 @@
         <v>202203748583.854</v>
       </c>
       <c r="U20" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>202.20374858385401</v>
       </c>
-      <c r="V20" s="212">
-        <f>K20</f>
+      <c r="V20" s="203">
+        <f t="shared" si="1"/>
         <v>9.3458836583736507E-2</v>
       </c>
-      <c r="W20" s="220">
-        <f t="shared" si="5"/>
+      <c r="W20" s="211">
+        <f t="shared" si="6"/>
         <v>18897727095.517353</v>
       </c>
       <c r="X20" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>18.897727095517354</v>
       </c>
       <c r="Y20" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.13507157931562963</v>
       </c>
-      <c r="Z20" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z20" s="205">
+        <f t="shared" si="2"/>
         <v>62.546500000000002</v>
       </c>
-      <c r="AA20" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA20" s="206">
+        <f t="shared" si="13"/>
         <v>3.1538306764169466E-2</v>
       </c>
     </row>
     <row r="21" spans="2:27" ht="15.75" customHeight="1">
       <c r="B21" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="C21" s="100">
@@ -25192,23 +25192,23 @@
         <v>14048256</v>
       </c>
       <c r="G21" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14048.255999999999</v>
       </c>
       <c r="I21" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.31301429667968472</v>
       </c>
       <c r="J21" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.13616560800089283</v>
       </c>
-      <c r="K21" s="219">
-        <f t="shared" si="3"/>
+      <c r="K21" s="210">
+        <f t="shared" si="4"/>
         <v>0.10800607562960129</v>
       </c>
       <c r="M21" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>16</v>
       </c>
       <c r="N21" s="123" t="s">
@@ -25218,11 +25218,11 @@
         <v>78.4983</v>
       </c>
       <c r="P21" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25503905094609602</v>
       </c>
       <c r="R21" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
       <c r="S21" s="123" t="s">
@@ -25232,37 +25232,37 @@
         <v>187337783856.466</v>
       </c>
       <c r="U21" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>187.33778385646599</v>
       </c>
-      <c r="V21" s="212">
-        <f>K21</f>
+      <c r="V21" s="203">
+        <f t="shared" si="1"/>
         <v>0.10800607562960129</v>
       </c>
-      <c r="W21" s="220">
-        <f t="shared" si="5"/>
+      <c r="W21" s="211">
+        <f t="shared" si="6"/>
         <v>20233618851.483368</v>
       </c>
       <c r="X21" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20.233618851483367</v>
       </c>
       <c r="Y21" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.0690604706790117E-2</v>
       </c>
-      <c r="Z21" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z21" s="205">
+        <f t="shared" si="2"/>
         <v>78.4983</v>
       </c>
-      <c r="AA21" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA21" s="206">
+        <f t="shared" si="13"/>
         <v>0.25503905094609602</v>
       </c>
     </row>
     <row r="22" spans="2:27" ht="15.75" customHeight="1">
       <c r="B22" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="C22" s="101">
@@ -25279,23 +25279,23 @@
         <v>15888604</v>
       </c>
       <c r="G22" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15888.603999999999</v>
       </c>
       <c r="I22" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.12437050887202705</v>
       </c>
       <c r="J22" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1310018837925504</v>
       </c>
-      <c r="K22" s="219">
-        <f t="shared" si="3"/>
+      <c r="K22" s="210">
+        <f t="shared" si="4"/>
         <v>0.10737280632080703</v>
       </c>
       <c r="M22" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>17</v>
       </c>
       <c r="N22" s="123" t="s">
@@ -25305,11 +25305,11 @@
         <v>83.801699999999997</v>
       </c>
       <c r="P22" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.7560698766724769E-2</v>
       </c>
       <c r="R22" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>17</v>
       </c>
       <c r="S22" s="123" t="s">
@@ -25319,37 +25319,37 @@
         <v>196709621849.586</v>
       </c>
       <c r="U22" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>196.709621849586</v>
       </c>
-      <c r="V22" s="212">
-        <f>K22</f>
+      <c r="V22" s="203">
+        <f t="shared" si="1"/>
         <v>0.10737280632080703</v>
       </c>
-      <c r="W22" s="220">
-        <f t="shared" si="5"/>
+      <c r="W22" s="211">
+        <f t="shared" si="6"/>
         <v>21121264128.294788</v>
       </c>
       <c r="X22" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>21.12126412829479</v>
       </c>
       <c r="Y22" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.3869822957861349E-2</v>
       </c>
       <c r="Z22" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.801699999999997</v>
       </c>
-      <c r="AA22" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA22" s="204">
+        <f t="shared" si="13"/>
         <v>6.7560698766724769E-2</v>
       </c>
     </row>
     <row r="23" spans="2:27" ht="14.4">
       <c r="B23" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="C23" s="101">
@@ -25366,23 +25366,23 @@
         <v>19102143</v>
       </c>
       <c r="G23" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19102.143</v>
       </c>
       <c r="I23" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.28688912804424849</v>
       </c>
       <c r="J23" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.20225433272803572</v>
       </c>
-      <c r="K23" s="219">
-        <f t="shared" si="3"/>
+      <c r="K23" s="210">
+        <f t="shared" si="4"/>
         <v>0.11493150271150206</v>
       </c>
       <c r="M23" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="N23" s="123" t="s">
@@ -25392,11 +25392,11 @@
         <v>85.5017</v>
       </c>
       <c r="P23" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.0285984651862599E-2</v>
       </c>
       <c r="R23" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
       <c r="S23" s="123" t="s">
@@ -25406,37 +25406,37 @@
         <v>230586581059.66501</v>
       </c>
       <c r="U23" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>230.58658105966501</v>
       </c>
-      <c r="V23" s="212">
-        <f>K23</f>
+      <c r="V23" s="203">
+        <f t="shared" si="1"/>
         <v>0.11493150271150206</v>
       </c>
-      <c r="W23" s="220">
-        <f t="shared" si="5"/>
+      <c r="W23" s="211">
+        <f t="shared" si="6"/>
         <v>26501662266.294876</v>
       </c>
       <c r="X23" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>26.501662266294876</v>
       </c>
       <c r="Y23" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.2547384524580758</v>
       </c>
-      <c r="Z23" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z23" s="205">
+        <f t="shared" si="2"/>
         <v>85.5017</v>
       </c>
-      <c r="AA23" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA23" s="206">
+        <f t="shared" si="13"/>
         <v>2.0285984651862599E-2</v>
       </c>
     </row>
     <row r="24" spans="2:27" ht="14.4">
       <c r="B24" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="C24" s="101">
@@ -25453,23 +25453,23 @@
         <v>21659650</v>
       </c>
       <c r="G24" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21659.65</v>
       </c>
       <c r="I24" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5687120292169499E-2</v>
       </c>
       <c r="J24" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.13388586819813875</v>
       </c>
-      <c r="K24" s="219">
-        <f t="shared" si="3"/>
+      <c r="K24" s="210">
+        <f t="shared" si="4"/>
         <v>9.4702638315946927E-2</v>
       </c>
       <c r="M24" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19</v>
       </c>
       <c r="N24" s="123" t="s">
@@ -25479,11 +25479,11 @@
         <v>89.235900000000001</v>
       </c>
       <c r="P24" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.3673985429529383E-2</v>
       </c>
       <c r="R24" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
       <c r="S24" s="123" t="s">
@@ -25493,37 +25493,37 @@
         <v>250106966104.70401</v>
       </c>
       <c r="U24" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>250.10696610470401</v>
       </c>
-      <c r="V24" s="212">
-        <f>K24</f>
+      <c r="V24" s="203">
+        <f t="shared" si="1"/>
         <v>9.4702638315946927E-2</v>
       </c>
-      <c r="W24" s="220">
-        <f t="shared" si="5"/>
+      <c r="W24" s="211">
+        <f t="shared" si="6"/>
         <v>23685789551.31258</v>
       </c>
       <c r="X24" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23.685789551312581</v>
       </c>
       <c r="Y24" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.10625268281995859</v>
       </c>
-      <c r="Z24" s="216">
-        <f t="shared" si="1"/>
+      <c r="Z24" s="207">
+        <f t="shared" si="2"/>
         <v>89.235900000000001</v>
       </c>
-      <c r="AA24" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA24" s="204">
+        <f t="shared" si="13"/>
         <v>4.3673985429529383E-2</v>
       </c>
     </row>
     <row r="25" spans="2:27" ht="14.4">
       <c r="B25" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="C25" s="99" t="s">
@@ -25540,23 +25540,23 @@
         <v>24159853</v>
       </c>
       <c r="G25" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24159.852999999999</v>
       </c>
       <c r="I25" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.11642549382661871</v>
       </c>
       <c r="J25" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.11543136661949749</v>
       </c>
-      <c r="K25" s="219">
-        <f t="shared" si="3"/>
+      <c r="K25" s="210">
+        <f t="shared" si="4"/>
         <v>9.4787041957581461E-2</v>
       </c>
       <c r="M25" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>20</v>
       </c>
       <c r="N25" s="123" t="s">
@@ -25566,11 +25566,11 @@
         <v>96.727199999999996</v>
       </c>
       <c r="P25" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8.3949397047600849E-2</v>
       </c>
       <c r="R25" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="S25" s="123" t="s">
@@ -25580,37 +25580,37 @@
         <v>258657231672.41199</v>
       </c>
       <c r="U25" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>258.65723167241197</v>
       </c>
-      <c r="V25" s="212">
-        <f>K25</f>
+      <c r="V25" s="203">
+        <f t="shared" si="1"/>
         <v>9.4787041957581461E-2</v>
       </c>
-      <c r="W25" s="220">
-        <f t="shared" si="5"/>
+      <c r="W25" s="211">
+        <f t="shared" si="6"/>
         <v>24517353871.164783</v>
       </c>
       <c r="X25" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.517353871164783</v>
       </c>
       <c r="Y25" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.5108152846275775E-2</v>
       </c>
       <c r="Z25" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96.727199999999996</v>
       </c>
-      <c r="AA25" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA25" s="204">
+        <f t="shared" si="13"/>
         <v>8.3949397047600849E-2</v>
       </c>
     </row>
     <row r="26" spans="2:27" ht="14.4">
       <c r="B26" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="C26" s="99" t="s">
@@ -25627,23 +25627,23 @@
         <v>26812907</v>
       </c>
       <c r="G26" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26812.906999999999</v>
       </c>
       <c r="I26" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.1499667473202444</v>
       </c>
       <c r="J26" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.10981250589562785</v>
       </c>
-      <c r="K26" s="219">
-        <f t="shared" si="3"/>
+      <c r="K26" s="210">
+        <f t="shared" si="4"/>
         <v>9.8216541757296216E-2</v>
       </c>
       <c r="M26" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>21</v>
       </c>
       <c r="N26" s="123" t="s">
@@ -25653,11 +25653,11 @@
         <v>102.8591</v>
       </c>
       <c r="P26" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.3393750671993043E-2</v>
       </c>
       <c r="R26" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>21</v>
       </c>
       <c r="S26" s="123" t="s">
@@ -25667,37 +25667,37 @@
         <v>271390474857.63199</v>
       </c>
       <c r="U26" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>271.390474857632</v>
       </c>
-      <c r="V26" s="212">
-        <f>K26</f>
+      <c r="V26" s="203">
+        <f t="shared" si="1"/>
         <v>9.8216541757296216E-2</v>
       </c>
-      <c r="W26" s="220">
-        <f t="shared" si="5"/>
+      <c r="W26" s="211">
+        <f t="shared" si="6"/>
         <v>26655033906.387062</v>
       </c>
       <c r="X26" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>26.655033906387061</v>
       </c>
       <c r="Y26" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.719048745861735E-2</v>
       </c>
-      <c r="Z26" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z26" s="205">
+        <f t="shared" si="2"/>
         <v>102.8591</v>
       </c>
-      <c r="AA26" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA26" s="206">
+        <f t="shared" si="13"/>
         <v>6.3393750671993043E-2</v>
       </c>
     </row>
     <row r="27" spans="2:27" ht="14.4">
       <c r="B27" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="C27" s="99" t="s">
@@ -25714,23 +25714,23 @@
         <v>29072548</v>
       </c>
       <c r="G27" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29072.547999999999</v>
       </c>
       <c r="I27" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.2557791598996189E-2</v>
       </c>
       <c r="J27" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.4274375769848531E-2</v>
       </c>
-      <c r="K27" s="219">
-        <f t="shared" si="3"/>
+      <c r="K27" s="210">
+        <f t="shared" si="4"/>
         <v>8.7633564144429313E-2</v>
       </c>
       <c r="M27" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>22</v>
       </c>
       <c r="N27" s="123" t="s">
@@ -25740,11 +25740,11 @@
         <v>101.29470000000001</v>
       </c>
       <c r="P27" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1.5209155048021894E-2</v>
       </c>
       <c r="R27" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>22</v>
       </c>
       <c r="S27" s="123" t="s">
@@ -25754,37 +25754,37 @@
         <v>299963590534.77301</v>
       </c>
       <c r="U27" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>299.963590534773</v>
       </c>
-      <c r="V27" s="212">
-        <f>K27</f>
+      <c r="V27" s="203">
+        <f t="shared" si="1"/>
         <v>8.7633564144429313E-2</v>
       </c>
-      <c r="W27" s="220">
-        <f t="shared" si="5"/>
+      <c r="W27" s="211">
+        <f t="shared" si="6"/>
         <v>26286878552.12236</v>
       </c>
       <c r="X27" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>26.28687855212236</v>
       </c>
       <c r="Y27" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-1.3811850908074907E-2</v>
       </c>
       <c r="Z27" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101.29470000000001</v>
       </c>
-      <c r="AA27" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA27" s="204">
+        <f t="shared" si="13"/>
         <v>-1.5209155048021894E-2</v>
       </c>
     </row>
     <row r="28" spans="2:27" ht="14.4">
       <c r="B28" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="C28" s="99" t="s">
@@ -25801,25 +25801,25 @@
         <v>30508205</v>
       </c>
       <c r="G28" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30508.205000000002</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.9852174346506768E-2</v>
       </c>
       <c r="J28" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.9381877364171878E-2</v>
       </c>
-      <c r="K28" s="219">
-        <f t="shared" si="3"/>
+      <c r="K28" s="210">
+        <f t="shared" si="4"/>
         <v>8.1851849363146725E-2</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>23</v>
       </c>
       <c r="N28" s="123" t="s">
@@ -25829,11 +25829,11 @@
         <v>104.2351</v>
       </c>
       <c r="P28" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.9028172253829698E-2</v>
       </c>
       <c r="R28" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
       <c r="S28" s="123" t="s">
@@ -25843,37 +25843,37 @@
         <v>313630000130.435</v>
       </c>
       <c r="U28" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>313.63000013043501</v>
       </c>
-      <c r="V28" s="212">
-        <f>K28</f>
+      <c r="V28" s="203">
+        <f t="shared" si="1"/>
         <v>8.1851849363146725E-2</v>
       </c>
-      <c r="W28" s="220">
-        <f t="shared" si="5"/>
+      <c r="W28" s="211">
+        <f t="shared" si="6"/>
         <v>25671195526.440052</v>
       </c>
       <c r="X28" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25.671195526440052</v>
       </c>
       <c r="Y28" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.342168639237685E-2</v>
       </c>
       <c r="Z28" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104.2351</v>
       </c>
-      <c r="AA28" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA28" s="204">
+        <f t="shared" si="13"/>
         <v>2.9028172253829698E-2</v>
       </c>
     </row>
     <row r="29" spans="2:27" ht="14.4">
       <c r="B29" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="C29" s="99" t="s">
@@ -25890,23 +25890,23 @@
         <v>33174970</v>
       </c>
       <c r="G29" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33174.97</v>
       </c>
       <c r="I29" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.12721327047241404</v>
       </c>
       <c r="J29" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.741140293242422E-2</v>
       </c>
-      <c r="K29" s="219">
-        <f t="shared" si="3"/>
+      <c r="K29" s="210">
+        <f t="shared" si="4"/>
         <v>8.48478235247839E-2</v>
       </c>
       <c r="M29" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="N29" s="123" t="s">
@@ -25916,11 +25916,11 @@
         <v>104.69710000000001</v>
       </c>
       <c r="P29" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.4322881639677902E-3</v>
       </c>
       <c r="R29" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>24</v>
       </c>
       <c r="S29" s="123" t="s">
@@ -25930,37 +25930,37 @@
         <v>339205534861.09998</v>
       </c>
       <c r="U29" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>339.20553486109998</v>
       </c>
-      <c r="V29" s="212">
-        <f>K29</f>
+      <c r="V29" s="203">
+        <f t="shared" si="1"/>
         <v>8.48478235247839E-2</v>
       </c>
-      <c r="W29" s="220">
-        <f t="shared" si="5"/>
+      <c r="W29" s="211">
+        <f t="shared" si="6"/>
         <v>28780851360.524544</v>
       </c>
       <c r="X29" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28.780851360524544</v>
       </c>
       <c r="Y29" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.12113404811558937</v>
       </c>
       <c r="Z29" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104.69710000000001</v>
       </c>
-      <c r="AA29" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA29" s="204">
+        <f t="shared" si="13"/>
         <v>4.4322881639677902E-3</v>
       </c>
     </row>
     <row r="30" spans="2:27" ht="14.4">
       <c r="B30" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="C30" s="99" t="s">
@@ -25977,23 +25977,23 @@
         <v>36514166</v>
       </c>
       <c r="G30" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36514.165999999997</v>
       </c>
       <c r="I30" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.4959301185438134E-2</v>
       </c>
       <c r="J30" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1006540774565885</v>
       </c>
-      <c r="K30" s="219">
-        <f t="shared" si="3"/>
+      <c r="K30" s="210">
+        <f t="shared" si="4"/>
         <v>8.209616508836598E-2</v>
       </c>
       <c r="M30" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25</v>
       </c>
       <c r="N30" s="123" t="s">
@@ -26003,11 +26003,11 @@
         <v>109.84439999999999</v>
       </c>
       <c r="P30" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.9163730418511964E-2</v>
       </c>
       <c r="R30" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>25</v>
       </c>
       <c r="S30" s="123" t="s">
@@ -26017,37 +26017,37 @@
         <v>356128166704.92102</v>
       </c>
       <c r="U30" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>356.128166704921</v>
       </c>
-      <c r="V30" s="212">
-        <f>K30</f>
+      <c r="V30" s="203">
+        <f t="shared" si="1"/>
         <v>8.209616508836598E-2</v>
       </c>
-      <c r="W30" s="220">
-        <f t="shared" si="5"/>
+      <c r="W30" s="211">
+        <f t="shared" si="6"/>
         <v>29236756766.424316</v>
       </c>
       <c r="X30" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>29.236756766424318</v>
       </c>
       <c r="Y30" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.5840580953942363E-2</v>
       </c>
       <c r="Z30" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109.84439999999999</v>
       </c>
-      <c r="AA30" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA30" s="204">
+        <f t="shared" si="13"/>
         <v>4.9163730418511964E-2</v>
       </c>
     </row>
     <row r="31" spans="2:27" ht="14.4">
       <c r="B31" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="C31" s="99" t="s">
@@ -26064,24 +26064,24 @@
         <v>41110164</v>
       </c>
       <c r="G31" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41110.163999999997</v>
       </c>
       <c r="I31" s="81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.58610228667367E-3</v>
       </c>
       <c r="J31" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1258689024966364</v>
       </c>
-      <c r="K31" s="219">
-        <f t="shared" si="3"/>
+      <c r="K31" s="210">
+        <f t="shared" si="4"/>
         <v>7.3617050031714787E-2</v>
       </c>
       <c r="L31" s="5"/>
       <c r="M31" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>26</v>
       </c>
       <c r="N31" s="123" t="s">
@@ -26091,12 +26091,12 @@
         <v>136.09010000000001</v>
       </c>
       <c r="P31" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.23893525750971389</v>
       </c>
       <c r="Q31" s="5"/>
       <c r="R31" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>26</v>
       </c>
       <c r="S31" s="123" t="s">
@@ -26106,37 +26106,37 @@
         <v>320909472770.66901</v>
       </c>
       <c r="U31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>320.90947277066903</v>
       </c>
-      <c r="V31" s="212">
-        <f>K31</f>
+      <c r="V31" s="203">
+        <f t="shared" si="1"/>
         <v>7.3617050031714787E-2</v>
       </c>
-      <c r="W31" s="220">
-        <f t="shared" si="5"/>
+      <c r="W31" s="211">
+        <f t="shared" si="6"/>
         <v>23624408712.609554</v>
       </c>
       <c r="X31" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23.624408712609554</v>
       </c>
       <c r="Y31" s="81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.19196205990467519</v>
       </c>
       <c r="Z31" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>136.09010000000001</v>
       </c>
-      <c r="AA31" s="213">
-        <f t="shared" si="12"/>
+      <c r="AA31" s="204">
+        <f t="shared" si="13"/>
         <v>0.23893525750971389</v>
       </c>
     </row>
     <row r="32" spans="2:27" ht="14.4">
       <c r="B32" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="C32" s="99" t="s">
@@ -26153,23 +26153,23 @@
         <v>44746876</v>
       </c>
       <c r="G32" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44746.875999999997</v>
       </c>
       <c r="I32" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.22397732758526701</v>
       </c>
       <c r="J32" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.8462600149199044E-2</v>
       </c>
-      <c r="K32" s="219">
-        <f t="shared" si="3"/>
+      <c r="K32" s="210">
+        <f t="shared" si="4"/>
         <v>8.2782449438481467E-2</v>
       </c>
       <c r="M32" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="N32" s="123" t="s">
@@ -26179,11 +26179,11 @@
         <v>158.02529999999999</v>
       </c>
       <c r="P32" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.16118145258178207</v>
       </c>
       <c r="R32" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>27</v>
       </c>
       <c r="S32" s="123" t="s">
@@ -26193,37 +26193,37 @@
         <v>300425609817.98102</v>
       </c>
       <c r="U32" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>300.42560981798101</v>
       </c>
-      <c r="V32" s="212">
-        <f>K32</f>
+      <c r="V32" s="203">
+        <f t="shared" si="1"/>
         <v>8.2782449438481467E-2</v>
       </c>
-      <c r="W32" s="220">
-        <f t="shared" si="5"/>
+      <c r="W32" s="211">
+        <f t="shared" si="6"/>
         <v>24869967854.781975</v>
       </c>
       <c r="X32" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.869967854781976</v>
       </c>
       <c r="Y32" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.272339965518813E-2</v>
       </c>
-      <c r="Z32" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z32" s="205">
+        <f t="shared" si="2"/>
         <v>158.02529999999999</v>
       </c>
-      <c r="AA32" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA32" s="206">
+        <f t="shared" si="13"/>
         <v>0.16118145258178207</v>
       </c>
     </row>
     <row r="33" spans="1:27" ht="14.4">
       <c r="B33" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="C33" s="99" t="s">
@@ -26240,23 +26240,23 @@
         <v>52254009</v>
       </c>
       <c r="G33" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52254.008999999998</v>
       </c>
       <c r="I33" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.27440679045940675</v>
       </c>
       <c r="J33" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.16776887396563733</v>
       </c>
-      <c r="K33" s="219">
-        <f t="shared" si="3"/>
+      <c r="K33" s="210">
+        <f t="shared" si="4"/>
         <v>9.0341948691439161E-2</v>
       </c>
       <c r="M33" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="N33" s="123" t="s">
@@ -26266,11 +26266,11 @@
         <v>160.02189999999999</v>
       </c>
       <c r="P33" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.263468571171833E-2</v>
       </c>
       <c r="R33" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>28</v>
       </c>
       <c r="S33" s="123" t="s">
@@ -26280,37 +26280,37 @@
         <v>348516647445.14801</v>
       </c>
       <c r="U33" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>348.51664744514801</v>
       </c>
-      <c r="V33" s="212">
-        <f>K33</f>
+      <c r="V33" s="203">
+        <f t="shared" si="1"/>
         <v>9.0341948691439161E-2</v>
       </c>
-      <c r="W33" s="220">
-        <f t="shared" si="5"/>
+      <c r="W33" s="211">
+        <f t="shared" si="6"/>
         <v>31485673081.601952</v>
       </c>
       <c r="X33" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>31.485673081601952</v>
       </c>
       <c r="Y33" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.26601181253830664</v>
       </c>
-      <c r="Z33" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z33" s="205">
+        <f t="shared" si="2"/>
         <v>160.02189999999999</v>
       </c>
-      <c r="AA33" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA33" s="206">
+        <f t="shared" si="13"/>
         <v>1.263468571171833E-2</v>
       </c>
     </row>
     <row r="34" spans="1:27" ht="14.4">
       <c r="B34" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="C34" s="99" t="s">
@@ -26327,23 +26327,23 @@
         <v>63305480</v>
       </c>
       <c r="G34" s="56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63305.48</v>
       </c>
       <c r="I34" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.22680458886752453</v>
       </c>
       <c r="J34" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.21149517925026573</v>
       </c>
-      <c r="K34" s="219">
-        <f t="shared" si="3"/>
+      <c r="K34" s="210">
+        <f t="shared" si="4"/>
         <v>9.1483580884308913E-2</v>
       </c>
       <c r="M34" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>29</v>
       </c>
       <c r="N34" s="123" t="s">
@@ -26353,11 +26353,11 @@
         <v>177.4512</v>
       </c>
       <c r="P34" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10891821681907299</v>
       </c>
       <c r="R34" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29</v>
       </c>
       <c r="S34" s="123" t="s">
@@ -26367,37 +26367,37 @@
         <v>374787958882.30798</v>
       </c>
       <c r="U34" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>374.78795888230798</v>
       </c>
-      <c r="V34" s="212">
-        <f>K34</f>
+      <c r="V34" s="203">
+        <f t="shared" si="1"/>
         <v>9.1483580884308913E-2</v>
       </c>
-      <c r="W34" s="220">
-        <f t="shared" si="5"/>
+      <c r="W34" s="211">
+        <f t="shared" si="6"/>
         <v>34286944550.874664</v>
       </c>
       <c r="X34" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34.286944550874665</v>
       </c>
       <c r="Y34" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.8969718449804391E-2</v>
       </c>
-      <c r="Z34" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z34" s="205">
+        <f t="shared" si="2"/>
         <v>177.4512</v>
       </c>
-      <c r="AA34" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA34" s="206">
+        <f t="shared" si="13"/>
         <v>0.10891821681907299</v>
       </c>
     </row>
     <row r="35" spans="1:27" ht="21" customHeight="1">
       <c r="B35" s="102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="C35" s="99" t="s">
@@ -26414,23 +26414,23 @@
         <v>79477291</v>
       </c>
       <c r="G35" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79477.290999999997</v>
       </c>
       <c r="I35" s="84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.3344643758724124</v>
       </c>
       <c r="J35" s="84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.25545673139197422</v>
       </c>
-      <c r="K35" s="219">
-        <f t="shared" si="3"/>
+      <c r="K35" s="210">
+        <f t="shared" si="4"/>
         <v>9.7240770322682496E-2</v>
       </c>
       <c r="M35" s="122">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="N35" s="123" t="s">
@@ -26440,11 +26440,11 @@
         <v>248.03</v>
       </c>
       <c r="P35" s="93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.39773639175164788</v>
       </c>
       <c r="R35" s="122">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>30</v>
       </c>
       <c r="S35" s="123" t="s">
@@ -26454,31 +26454,31 @@
         <v>338368455317.87598</v>
       </c>
       <c r="U35" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>338.368455317876</v>
       </c>
-      <c r="V35" s="212">
-        <f>K35</f>
+      <c r="V35" s="203">
+        <f t="shared" si="1"/>
         <v>9.7240770322682496E-2</v>
       </c>
-      <c r="W35" s="220">
-        <f t="shared" si="5"/>
+      <c r="W35" s="211">
+        <f t="shared" si="6"/>
         <v>32903209248.006432</v>
       </c>
       <c r="X35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>32.903209248006434</v>
       </c>
       <c r="Y35" s="84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-4.0357498196290309E-2</v>
       </c>
-      <c r="Z35" s="214">
-        <f t="shared" si="1"/>
+      <c r="Z35" s="205">
+        <f t="shared" si="2"/>
         <v>248.03</v>
       </c>
-      <c r="AA35" s="215">
-        <f t="shared" si="12"/>
+      <c r="AA35" s="206">
+        <f t="shared" si="13"/>
         <v>0.39773639175164788</v>
       </c>
     </row>
@@ -26523,13 +26523,13 @@
         <v>7.0272629959299504E-2</v>
       </c>
       <c r="W37" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="X37" s="88">
         <f>((X34/X6)^(1/29))-1</f>
         <v>5.3440888730394098E-2</v>
       </c>
-      <c r="Y37" s="217"/>
+      <c r="Y37" s="208"/>
       <c r="Z37" s="88">
         <f>((Z34/Z6)^(1/29))-1</f>
         <v>6.3010821769164505E-2</v>
@@ -26608,7 +26608,7 @@
         <v>5</v>
       </c>
       <c r="C45" s="92" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -26646,17 +26646,17 @@
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="218" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207" t="s">
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="207"/>
+      <c r="G2" s="218"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="94"/>
@@ -31079,12 +31079,12 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="17.399999999999999">
-      <c r="C3" s="207" t="s">
+      <c r="C3" s="218" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="218"/>
+      <c r="F3" s="218"/>
     </row>
     <row r="4" spans="2:6" ht="13.2">
       <c r="C4" s="6" t="s">
@@ -31814,15 +31814,15 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:27" ht="18">
-      <c r="C2" s="208" t="s">
+      <c r="C2" s="217" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
+      <c r="I2" s="217"/>
     </row>
     <row r="3" spans="2:27" ht="14.4">
       <c r="C3" s="30" t="s">
@@ -32779,10 +32779,10 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="2:6" ht="18">
-      <c r="C2" s="205" t="s">
+      <c r="C2" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="205"/>
+      <c r="D2" s="215"/>
     </row>
     <row r="3" spans="2:6" ht="14.4">
       <c r="C3" s="17" t="s">
@@ -33429,13 +33429,13 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:7" ht="18">
-      <c r="C2" s="205" t="s">
+      <c r="C2" s="215" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="205"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" customHeight="1">
       <c r="C3" s="17" t="s">

</xml_diff>

<commit_message>
Added analysis for regression and completed tables
</commit_message>
<xml_diff>
--- a/data/Report - Data Tables Ver4_Fin_SA 072724.xlsx
+++ b/data/Report - Data Tables Ver4_Fin_SA 072724.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sifaat\FFC-Forecasting-Study\forecasting-study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE6AED-3CA9-4ABF-9EB2-AD67CD9862A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143F364-401D-431C-92D2-3EEF8021CBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,6 +686,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -693,41 +694,48 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF980000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -738,6 +746,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -804,6 +813,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -867,6 +877,7 @@
       <sz val="10"/>
       <color rgb="FF0070C0"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1600,6 +1611,7 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1625,7 +1637,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2420,13 +2431,13 @@
         <c:crossAx val="2083197936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="500"/>
+        <c:minorUnit val="500"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="2086241648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="400"/>
+          <c:max val="150"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2520,7 +2531,7 @@
         <c:crossAx val="2086242128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="50"/>
+        <c:majorUnit val="25"/>
       </c:valAx>
       <c:catAx>
         <c:axId val="2086242128"/>
@@ -3414,10 +3425,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:N63"/>
+  <dimension ref="B1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -3451,13 +3462,13 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="214" t="s">
+      <c r="H2" s="215" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="214"/>
-      <c r="J2" s="215"/>
-      <c r="K2" s="215"/>
-      <c r="L2" s="215"/>
+      <c r="I2" s="215"/>
+      <c r="J2" s="216"/>
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
@@ -4860,7 +4871,7 @@
         <v>147433.07462686568</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="14.4">
+    <row r="33" spans="2:15" ht="14.4">
       <c r="B33" s="21">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4908,8 +4919,9 @@
         <f>'6. Technology Proxy'!F33</f>
         <v>187479.30897537729</v>
       </c>
-    </row>
-    <row r="34" spans="2:13" ht="14.4">
+      <c r="O33" s="46"/>
+    </row>
+    <row r="34" spans="2:15" ht="14.4">
       <c r="B34" s="21">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4957,8 +4969,12 @@
         <f>'6. Technology Proxy'!F34</f>
         <v>229453.72424722664</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" ht="15.75" customHeight="1">
+      <c r="O34" s="46">
+        <f>0.01*I34</f>
+        <v>0.34286944550874665</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" ht="15.75" customHeight="1">
       <c r="B35" s="21">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5007,7 +5023,7 @@
         <v>305592.44760775013</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="15.75" customHeight="1">
+    <row r="36" spans="2:15" ht="15.75" customHeight="1">
       <c r="J36" s="46">
         <f>$K$36 -$K$37</f>
         <v>0.8811548786009451</v>
@@ -5021,8 +5037,8 @@
         <v>1.041154878600945</v>
       </c>
     </row>
-    <row r="37" spans="2:13" ht="15.75" customHeight="1">
-      <c r="K37" s="223">
+    <row r="37" spans="2:15" ht="15.75" customHeight="1">
+      <c r="K37" s="214">
         <f>0.08</f>
         <v>0.08</v>
       </c>
@@ -5072,17 +5088,17 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="2:11" ht="18">
-      <c r="C2" s="220" t="s">
+      <c r="C2" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
     </row>
     <row r="3" spans="2:11" ht="14.4">
       <c r="C3" s="15" t="s">
@@ -6437,36 +6453,36 @@
       <c r="X1" s="18"/>
     </row>
     <row r="2" spans="2:29" ht="18">
-      <c r="C2" s="221" t="s">
+      <c r="C2" s="222" t="s">
         <v>158</v>
       </c>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="221"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221"/>
-      <c r="J2" s="221"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
-      <c r="M2" s="221"/>
-      <c r="N2" s="221"/>
-      <c r="O2" s="221"/>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="221"/>
-      <c r="R2" s="221"/>
-      <c r="S2" s="221"/>
-      <c r="T2" s="221"/>
-      <c r="U2" s="221"/>
-      <c r="V2" s="221"/>
-      <c r="W2" s="221"/>
-      <c r="X2" s="221"/>
-      <c r="Z2" s="218" t="s">
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
+      <c r="Q2" s="222"/>
+      <c r="R2" s="222"/>
+      <c r="S2" s="222"/>
+      <c r="T2" s="222"/>
+      <c r="U2" s="222"/>
+      <c r="V2" s="222"/>
+      <c r="W2" s="222"/>
+      <c r="X2" s="222"/>
+      <c r="Z2" s="219" t="s">
         <v>93</v>
       </c>
-      <c r="AA2" s="218"/>
-      <c r="AB2" s="218"/>
-      <c r="AC2" s="218"/>
+      <c r="AA2" s="219"/>
+      <c r="AB2" s="219"/>
+      <c r="AC2" s="219"/>
     </row>
     <row r="3" spans="2:29" ht="14.4">
       <c r="C3" s="25" t="s">
@@ -19207,14 +19223,14 @@
       <c r="D1" s="14"/>
     </row>
     <row r="2" spans="2:7" ht="18">
-      <c r="B2" s="218" t="s">
+      <c r="B2" s="219" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
     </row>
     <row r="3" spans="2:7" ht="18">
       <c r="B3" s="93"/>
@@ -20032,13 +20048,13 @@
       <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="18">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="219" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
     </row>
     <row r="3" spans="1:5" s="23" customFormat="1" ht="14.4">
       <c r="C3" s="26" t="s">
@@ -20486,11 +20502,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="14.4">
-      <c r="B3" s="222" t="s">
+      <c r="B3" s="223" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
+      <c r="C3" s="223"/>
+      <c r="D3" s="223"/>
     </row>
     <row r="4" spans="2:4" ht="43.2">
       <c r="B4" s="32" t="s">
@@ -20910,11 +20926,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="14.4">
-      <c r="B3" s="222" t="s">
+      <c r="B3" s="223" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
+      <c r="C3" s="223"/>
+      <c r="D3" s="223"/>
     </row>
     <row r="4" spans="2:4" ht="57.6">
       <c r="B4" s="32" t="s">
@@ -21337,12 +21353,12 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="18">
-      <c r="C3" s="216" t="s">
+      <c r="C3" s="217" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
     </row>
     <row r="4" spans="2:6" ht="14.4">
       <c r="C4" s="17" t="s">
@@ -24925,14 +24941,14 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="18">
-      <c r="A3" s="216" t="s">
+      <c r="A3" s="217" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="216"/>
-      <c r="C3" s="216"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
+      <c r="B3" s="217"/>
+      <c r="C3" s="217"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
     </row>
     <row r="4" spans="1:6" ht="14.4">
       <c r="C4" s="17" t="s">
@@ -25498,38 +25514,38 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:27" ht="18">
-      <c r="C3" s="216" t="s">
+      <c r="C3" s="217" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
-      <c r="I3" s="216" t="s">
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
+      <c r="I3" s="217" t="s">
         <v>121</v>
       </c>
-      <c r="J3" s="216"/>
-      <c r="K3" s="216"/>
-      <c r="N3" s="218" t="s">
+      <c r="J3" s="217"/>
+      <c r="K3" s="217"/>
+      <c r="N3" s="219" t="s">
         <v>171</v>
       </c>
-      <c r="O3" s="218"/>
-      <c r="P3" s="218"/>
-      <c r="S3" s="218" t="s">
+      <c r="O3" s="219"/>
+      <c r="P3" s="219"/>
+      <c r="S3" s="219" t="s">
         <v>172</v>
       </c>
-      <c r="T3" s="218"/>
-      <c r="U3" s="218"/>
-      <c r="V3" s="218"/>
-      <c r="W3" s="218"/>
-      <c r="X3" s="218"/>
-      <c r="Y3" s="218"/>
-      <c r="Z3" s="218"/>
+      <c r="T3" s="219"/>
+      <c r="U3" s="219"/>
+      <c r="V3" s="219"/>
+      <c r="W3" s="219"/>
+      <c r="X3" s="219"/>
+      <c r="Y3" s="219"/>
+      <c r="Z3" s="219"/>
     </row>
     <row r="4" spans="2:27" ht="14.4">
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="218" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="217"/>
+      <c r="C4" s="218"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="I4" s="53" t="s">
@@ -28444,17 +28460,17 @@
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="A2" s="219" t="s">
+      <c r="A2" s="220" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219" t="s">
+      <c r="B2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="219"/>
+      <c r="G2" s="220"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="92"/>
@@ -32877,12 +32893,12 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="2:6" ht="17.399999999999999">
-      <c r="C3" s="219" t="s">
+      <c r="C3" s="220" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
     </row>
     <row r="4" spans="2:6" ht="13.2">
       <c r="C4" s="6" t="s">
@@ -33612,15 +33628,15 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="2:27" ht="18">
-      <c r="C2" s="218" t="s">
+      <c r="C2" s="219" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="218"/>
-      <c r="I2" s="218"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
     </row>
     <row r="3" spans="2:27" ht="14.4">
       <c r="C3" s="28" t="s">
@@ -34577,10 +34593,10 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="2:6" ht="18">
-      <c r="C2" s="216" t="s">
+      <c r="C2" s="217" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="216"/>
+      <c r="D2" s="217"/>
     </row>
     <row r="3" spans="2:6" ht="14.4">
       <c r="C3" s="17" t="s">
@@ -35227,13 +35243,13 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="2:7" ht="18">
-      <c r="C2" s="216" t="s">
+      <c r="C2" s="217" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" customHeight="1">
       <c r="C3" s="17" t="s">

</xml_diff>